<commit_message>
Band Gap lab report is near to complete
</commit_message>
<xml_diff>
--- a/Solid_State_Electronics_Labs/Band gap/data.xlsx
+++ b/Solid_State_Electronics_Labs/Band gap/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexn\Documents\GitHub\Labs\Solid_State_Electronics_Labs\Band gap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BFC857-84AC-4482-AFD0-222FB265A9F9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F9BC22-6A9F-46ED-B7AD-5C0FC3D427ED}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" activeTab="1" xr2:uid="{6F31562E-81D9-4544-A5C7-2A6C2D640A1F}"/>
+    <workbookView xWindow="14783" yWindow="2325" windowWidth="18194" windowHeight="14175" xr2:uid="{6F31562E-81D9-4544-A5C7-2A6C2D640A1F}"/>
   </bookViews>
   <sheets>
     <sheet name="CdSe" sheetId="1" r:id="rId1"/>
@@ -3583,6 +3583,71 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>475620</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>163260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>28980</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>3660</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="6" name="Рукописный ввод 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA33082C-428E-4E6A-A87E-063F765013C3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8248020" y="8488110"/>
+            <a:ext cx="2144160" cy="2736000"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="6" name="Рукописный ввод 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA33082C-428E-4E6A-A87E-063F765013C3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8239380" y="8479470"/>
+              <a:ext cx="2161800" cy="2753640"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3637,8 +3702,8 @@
       <xdr:row>53</xdr:row>
       <xdr:rowOff>140145</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="13" name="Рукописный ввод 12">
@@ -3657,7 +3722,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="13" name="Рукописный ввод 12">
@@ -3693,6 +3758,38 @@
 </file>
 
 <file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2019-02-10T01:14:15.971"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">5956 1 1544 0 0,'-9'21'674'0'0,"-1"0"-1"0"0,-7 11-673 0 0,4-10 650 0 0,2 2 1 0 0,-1 2-651 0 0,-6 21 179 0 0,-9 36 130 0 0,23-74-150 0 0,1 0 1 0 0,-2-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,-1-1-159 0 0,-10 16 317 0 0,-37 46 331 0 0,18-19 40 0 0,-9 14-792 0 0,23-35 226 0 0,-1 2 244 0 0,15-19-3 0 0,0 0-1 0 0,-11 11-362 0 0,10-12 153 0 0,-67 74 542 0 0,36-42-476 0 0,-30 25-59 0 0,28-29-106 0 0,29-24 28 0 0,-2 2 174 0 0,0 0 0 0 0,-8 14-256 0 0,3-5 252 0 0,14-20-16 0 0,1 1 0 0 0,0-1 0 0 0,-5 8-236 0 0,-17 28 281 0 0,19-31-216 0 0,0 0 0 0 0,1 1 0 0 0,1 0 0 0 0,-4 7-65 0 0,6-10 2 0 0,0 0 0 0 0,-1-1-1 0 0,-5 7-1 0 0,5-7 27 0 0,0-1-1 0 0,1 1 0 0 0,-3 6-26 0 0,4-6 15 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,0 0 1 0 0,0-1-1 0 0,-2 3-15 0 0,-3 1 61 0 0,1 0 0 0 0,0 1 0 0 0,-1 3-61 0 0,0-1 68 0 0,-1 0-1 0 0,-4 4-67 0 0,3-5 35 0 0,-10 11 152 0 0,0-1-1 0 0,-2 0 1 0 0,-22 14-187 0 0,29-27 39 0 0,14-9-34 0 0,-1 2 0 0 0,1-1 1 0 0,0 0-1 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 2-5 0 0,-47 45 74 0 0,46-43-17 0 0,0-1 0 0 0,0 1 1 0 0,0 0-1 0 0,1 0 0 0 0,-4 6-57 0 0,-6 10 158 0 0,-6 5-76 0 0,-8 18-82 0 0,10-15 0 0 0,-16 33 2 0 0,22-38 69 0 0,-44 99 104 0 0,24-71-175 0 0,25-41 0 0 0,-1 1 0 0 0,-1-2 0 0 0,0 1 0 0 0,-6 5 0 0 0,7-8 0 0 0,-18 18 10 0 0,17-19 31 0 0,1 1 0 0 0,0-1 0 0 0,-3 5-41 0 0,-2 2 114 0 0,0 0 0 0 0,-13 11-114 0 0,-10 12 164 0 0,29-31-138 0 0,0 1 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 1 0 0,0 2-27 0 0,-30 46 64 0 0,29-43-44 0 0,-1 0 1 0 0,-1-1 0 0 0,-1 0-21 0 0,1 0 0 0 0,1 0 1 0 0,0 0 0 0 0,0 2-1 0 0,-15 27 53 0 0,17-34-47 0 0,1 1 0 0 0,-1 0 1 0 0,0-1-1 0 0,-1 0 0 0 0,1 0 0 0 0,-1-1 1 0 0,0 0-1 0 0,-5 3-6 0 0,3-1 58 0 0,0 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-2 3-59 0 0,-72 83 606 0 0,14-15-256 0 0,28-34-410 0 0,-6 4 60 0 0,39-41 0 0 0,1-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,-3 1 0 0 0,3-2 0 0 0,-1 1 0 0 0,2 0 0 0 0,-1 0 0 0 0,-1 3 0 0 0,-65 78 197 0 0,10-8-48 0 0,-23 40 164 0 0,75-105-270 0 0,-6 8 38 0 0,2-7 29 0 0,1 1 0 0 0,0 1 0 0 0,1 0 0 0 0,1 0 0 0 0,-4 8-110 0 0,12-20 71 0 0,0-1-1 0 0,0 0 1 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,-1 0-71 0 0,1 0-40 0 0,0 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 3 40 0 0,-18 26-109 0 0,4-5 465 0 0,-7 13-356 0 0,17-27-35 0 0,0 0 0 0 0,-1-1-1 0 0,-11 10 36 0 0,-15 21 145 0 0,0-4 1 0 0,28-32-160 0 0,6-6 3 0 0,0 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-2 2 11 0 0,2-1 8 0 0,-2 0-1 0 0,1 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-1-1 1 0 0,0 1-1 0 0,1-1 0 0 0,-4 2-7 0 0,-15 13-1 0 0,-21 31 65 0 0,29-37-77 0 0,-5 6-24 0 0,0 9 143 0 0,-35 47 118 0 0,39-57-205 0 0,7-9-1 0 0,0 0 1 0 0,1 1 0 0 0,-3 6-19 0 0,1-1 45 0 0,6-8-44 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1-1 0 0 0,-1 1 0 0 0,0-1 0 0 0,-3 3-1 0 0,2-3 0 0 0,1-1 0 0 0,1 2 0 0 0,-1-1 0 0 0,0 0 0 0 0,1 1 0 0 0,0-1 0 0 0,0 1 0 0 0,1 0 0 0 0,-2 2 0 0 0,-15 24 0 0 0,-8 7 0 0 0,13-18 0 0 0,10-13 0 0 0,-1 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,-4 3 0 0 0,-24 30 54 0 0,10-15 24 0 0,19-19-79 0 0,-1-1 0 0 0,0 0 1 0 0,0 0-1 0 0,0 0 1 0 0,-1 0-1 0 0,-4 2 1 0 0,-20 20 0 0 0,15-11 0 0 0,10-12 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-3 4 0 0 0,2-3 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 0 0 0 0,1-1 0 0 0,1-1 0 0 0,0 1 0 0 0,0 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,1-1 0 0 0,-3 2 0 0 0,3-2 0 0 0,-1 0 0 0 0,1-1 0 0 0,0 2 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 1 0 0 0,1-2 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 0 0 0 0,0-1 0 0 0,-1 2 0 0 0,-5 2 72 0 0,-1 1 0 0 0,1 1-1 0 0,0 0 1 0 0,1 0 0 0 0,-1 0-1 0 0,1 1 1 0 0,1 0 0 0 0,-5 7-72 0 0,-1 2-359 0 0,7-9 499 0 0,0 0 1 0 0,0 0-1 0 0,-3 8-140 0 0,4-9-114 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-4 4 114 0 0,-13 20-84 0 0,-51 97 84 0 0,70-122 0 0 0,-4 5 0 0 0,1 0 0 0 0,-2 0 0 0 0,1-1 0 0 0,-9 10 0 0 0,11-11 0 0 0,-2-2 0 0 0,1 1 0 0 0,-1 0 0 0 0,-2 1 0 0 0,-11 14 0 0 0,16-18 0 0 0,1-1 0 0 0,0 0 0 0 0,-1 0 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,-2 2 0 0 0,3-2 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,-1-2 0 0 0,-2 2 0 0 0,-21 21 0 0 0,-9 1 0 0 0,23-17 98 0 0,1 0-1 0 0,0 0 0 0 0,1 1 1 0 0,0 1-1 0 0,0 0 0 0 0,-8 11-97 0 0,10-9 0 0 0,0 1 0 0 0,-2 6 0 0 0,4-8 0 0 0,1-1 0 0 0,-1 0 0 0 0,-1-1 0 0 0,-1 2 0 0 0,-27 40 0 0 0,-14 16 0 0 0,35-42 0 0 0,13-20 0 0 0,-1 0 0 0 0,0-1 0 0 0,-1 0 0 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-2 4 0 0 0,3-4 0 0 0,0-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0-1 0 0 0,-3 4 0 0 0,-16 19-329 0 0,-32 31 50 0 0,22-27 299 0 0,-22 28-20 0 0,-22 35 588 0 0,-18 12-588 0 0,86-96 0 0 0,-27 33 0 0 0,-11 21 0 0 0,34-47-7 0 0,0-1-1 0 0,-6 5 8 0 0,2-2-185 0 0,-4 5 289 0 0,-1-1 0 0 0,-13 11-104 0 0,11-5-85 0 0,-8 11 32 0 0,23-31 92 0 0,1 2 0 0 0,0-1 0 0 0,0 1 0 0 0,0 2-39 0 0,-11 15-2 0 0,-5 10 2 0 0,17-25 0 0 0,-1 0 0 0 0,-6 6 0 0 0,-9 15-56 0 0,15-23-3 0 0,1 0 1 0 0,-2 0-1 0 0,-6 7 59 0 0,3-5 80 0 0,0 1 1 0 0,1 0-1 0 0,-3 6-80 0 0,6-7-2 0 0,-1-1 0 0 0,0-1-1 0 0,-1 1 1 0 0,-8 6 2 0 0,-33 40 0 0 0,38-47 0 0 0,8-7 0 0 0,1 0 0 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,1 1 0 0 0,-3 2 0 0 0,-8 11-53 0 0,1-2 0 0 0,-2 0 0 0 0,-4 4 53 0 0,1-2 74 0 0,1 0-1 0 0,-5 10-73 0 0,10-13-24 0 0,1 0-15 0 0,1-1-1 0 0,0 1 1 0 0,-2 6 39 0 0,-20 28 61 0 0,25-39-106 0 0,0 0 0 0 0,-1-1 0 0 0,0 1 0 0 0,-7 6 45 0 0,6-8 33 0 0,1 1 1 0 0,0 0-1 0 0,1 0 0 0 0,0 1 1 0 0,0-1-1 0 0,1 1-33 0 0,-3 5 10 0 0,-1-2 0 0 0,-1 1-1 0 0,0-1 1 0 0,0-1 0 0 0,-1 0 0 0 0,-1 0-1 0 0,-3 1-9 0 0,7-4 5 0 0,-16 12-5 0 0,-17 10 0 0 0,18-13 0 0 0,-33 35 0 0 0,36-36 0 0 0,1 2 0 0 0,1 0 0 0 0,0 1 0 0 0,-3 7 0 0 0,-60 87 0 0 0,59-78-180 0 0,-8 19 180 0 0,9-15-1220 0 0,-5 3 1220 0 0,-27 45-1879 0 0,36-58 1175 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3220.067">629 6810 5648 0 0,'-5'0'288'0'0,"-11"-7"560"0"0,15 6-584 0 0,1 0-171 0 0,-1 0-28 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,1 0 0 0 0,-1-1 0 0 0,0 1 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 0 0 0,-1-1 0 0 0,1 1 1 0 0,0-1-1 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0 0 0 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 1-65 0 0,1-14 2009 0 0,-2 15-1892 0 0,0-1 1 0 0,0 1-1 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 1 0 0,-1-1-1 0 0,1 1 0 0 0,0 0 0 0 0,0-1 0 0 0,0 1 0 0 0,-1-1 0 0 0,1 1 0 0 0,0 0 1 0 0,0-1-1 0 0,-1 1 0 0 0,1 0 0 0 0,0-1 0 0 0,-1 1-117 0 0,0-1 156 0 0,-1 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 1 0 0 0,1-1 0 0 0,-1 1 0 0 0,0 0 0 0 0,1 0-1 0 0,-1-1 1 0 0,0 1 0 0 0,1 0 0 0 0,-2 1-156 0 0,1-1 6 0 0,1 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,0 1 1 0 0,1-1-1 0 0,-1 1 1 0 0,0-1-1 0 0,0 1 1 0 0,1 0-1 0 0,-1-1 1 0 0,1 1-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 1-1 0 0,0-1 1 0 0,-1 0-1 0 0,1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 1 0 0,-1 2-6 0 0,1 0 3 0 0,-1-1-1 0 0,1 1 1 0 0,0 0 0 0 0,0 0 0 0 0,1 0-1 0 0,-1-1 1 0 0,0 1 0 0 0,1 0 0 0 0,0 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,0 2-3 0 0,2 7 0 0 0,-2 0 0 0 0,0 1 0 0 0,-1 10 0 0 0,0 8 0 0 0,-5 29 0 0 0,5-47 206 0 0,0 0 1 0 0,-1-1 0 0 0,-1 1-1 0 0,0 0 1 0 0,-1-1 0 0 0,-1 0-1 0 0,1 0 1 0 0,-2 0 0 0 0,0 0-207 0 0,-2 6 81 0 0,4-8-164 0 0,8-13 210 0 0,8-16 83 0 0,-11 17-195 0 0,2-5 69 0 0,0 0 0 0 0,0-1 0 0 0,-1 1 1 0 0,0-1-1 0 0,-1 1 0 0 0,0-1 0 0 0,1-6-84 0 0,0-3 147 0 0,-1 14-116 0 0,0 0-1 0 0,-1 0 1 0 0,0 0-1 0 0,1 0 0 0 0,-1-1 1 0 0,0 1-1 0 0,-1-1-30 0 0,-12-95 744 0 0,8 89-632 0 0,4 9-84 0 0,0-1-1 0 0,1 1 1 0 0,-1 0-1 0 0,0-1 0 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1-1-1 0 0,1 0 1 0 0,0 1-1 0 0,0-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0-1-27 0 0,7 25 16 0 0,-4-6-16 0 0,-1 0 0 0 0,0 15 0 0 0,0 1 0 0 0,11 64 75 0 0,-12-76-16 0 0,-2-17-40 0 0,1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,1 1 0 0 0,-1 0 0 0 0,0-1 0 0 0,1 1-1 0 0,0-1 1 0 0,0 1-19 0 0,-1-1 75 0 0,0-2-2 0 0,0 3 11 0 0,0-2 3 0 0,0-1 6 0 0,0 0 43 0 0,0 0-4 0 0,1-2-4 0 0,3-11-38 0 0,0 0 0 0 0,-1 1 1 0 0,-1-1-1 0 0,0 0 0 0 0,0-1 0 0 0,-2 1 0 0 0,1-2-90 0 0,2-37 49 0 0,0 19-21 0 0,-2 1-1 0 0,-3-15-27 0 0,1-2 20 0 0,0 40 23 0 0,-1 5-33 0 0,1 7-9 0 0,0 7-2 0 0,6 53 1 0 0,-4-31-3 0 0,-1-3 2 0 0,0 1 0 0 0,-2-1 0 0 0,-3 9 1 0 0,2-29 16 0 0,2-7-24 0 0,0 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 2 8 0 0,0-3 88 0 0,0-1-3 0 0,2-17 131 0 0,-1 4-144 0 0,3-20 220 0 0,-2 0 0 0 0,-2 0 0 0 0,-3-27-292 0 0,1-17 286 0 0,2 73-343 0 0,0-1 1 0 0,0 1 0 0 0,1-1 0 0 0,-1 0 0 0 0,1 1 0 0 0,0-1 0 0 0,1 1-1 0 0,-1 0 1 0 0,1-2 56 0 0,-1 4 94 0 0,-1 2 118 0 0,0 0 20 0 0,0 0-60 0 0,2 5-502 0 0,0-2 284 0 0,0 0 0 0 0,0 1 0 0 0,0-1 0 0 0,-1 0-1 0 0,1 1 1 0 0,-1-1 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1-1 0 0,0 0 1 0 0,0 1 46 0 0,11 47 0 0 0,-6-21 0 0 0,-3-24 0 0 0,-2 0 0 0 0,1 1 0 0 0,-1-1 0 0 0,0 7 0 0 0,3 117 98 0 0,-4-130 71 0 0,0-1 44 0 0,0 0 3 0 0,0 0-54 0 0,0 0-230 0 0,0 0-100 0 0,0 0-22 0 0,1-1 50 0 0,0-5 202 0 0,1 0 1 0 0,-1 0-1 0 0,0 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0-62 0 0,1-28-132 0 0,2 9 44 0 0,-1 0 0 0 0,-1-1 0 0 0,-3-24 88 0 0,-1-4 61 0 0,3-31-61 0 0,1 64 3 0 0,1 9-3 0 0,1 23-32 0 0,-1 11 0 0 0,-5 88 32 0 0,-1 30 0 0 0,2-113 0 0 0,-1 0 0 0 0,-4 11 0 0 0,-3 19 0 0 0,6-33 43 0 0,-6 18-43 0 0,0-1 21 0 0,1-7 191 0 0,5-21-66 0 0,3-10-98 0 0,1-5-30 0 0,3-20-18 0 0,1 0 0 0 0,0 0 0 0 0,2 0 0 0 0,0 1 0 0 0,5-11 0 0 0,8-34 0 0 0,-10 31-393 0 0,1 0-1 0 0,2 1 0 0 0,13-31 394 0 0,-18 54-1309 0 0,3 5-377 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -4028,8 +4125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{145C4C2F-9081-45E6-AA35-19356AA9F138}">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView topLeftCell="E40" workbookViewId="0">
-      <selection activeCell="U49" sqref="U49"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6068,7 +6165,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6076,8 +6174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A50FC5-D451-438E-AD09-DB73B8A59F25}">
   <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="J58" sqref="J58"/>
+    <sheetView topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>